<commit_message>
allow aster to chose as long as he wants
allow aster to chose as long as he wants
</commit_message>
<xml_diff>
--- a/MySmartLock/MySmartLocker.xlsx
+++ b/MySmartLock/MySmartLocker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saaamar\Documents\GitHub\SmartLocker\MySmartLock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AA993-1065-4F85-B375-AEFD77113D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC9260E-AEF4-43CC-AAFF-9B251E0251B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54735" yWindow="8265" windowWidth="28800" windowHeight="13545" xr2:uid="{332520F4-A6D1-49F8-BAAA-23A5BE170209}"/>
   </bookViews>
@@ -590,7 +590,7 @@
       </c>
       <c r="K4" t="str">
         <f ca="1" xml:space="preserve"> TEXT(NOW(),"yyyymmddhh")</f>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M4" t="str">
         <f ca="1">CONCATENATE(C4,D4,E4,F4,G4,H4,I4)</f>
@@ -598,20 +598,20 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N5" ca="1" si="1">$J4+$K4+$M4+Q$10</f>
-        <v>2027189643</v>
+        <v>2024360337</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O7" ca="1" si="2">$J4*$K4+$M4+R$10</f>
-        <v>2031516233</v>
+        <f t="shared" ref="O4" ca="1" si="2">$J4*$K4+$M4+R$10</f>
+        <v>2022725278</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:R4" ca="1" si="3">MOD(N4,$B$2)</f>
-        <v>13916173</v>
+        <v>11086867</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>2756044</v>
+        <v>9451808</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K7" ca="1" si="7" xml:space="preserve"> TEXT(NOW(),"yyyymmddhh")</f>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M5" t="str">
         <f ca="1">CONCATENATE(C5,D5,E5,F5,G5,H5,I5)</f>
@@ -663,20 +663,20 @@
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="1"/>
-        <v>2038854642</v>
+        <v>2036025336</v>
       </c>
       <c r="O5">
         <f ca="1">$J5*$K5+$M5+R$10</f>
-        <v>2020115796524</v>
+        <v>2020107007567</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="4">
         <f ca="1">MOD(N5,$B$2)</f>
-        <v>10094453</v>
+        <v>7265147</v>
       </c>
       <c r="R5" s="4">
         <f ca="1">MOD(O5,$B$2)</f>
-        <v>12683445</v>
+        <v>3894488</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -716,12 +716,11 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J5:J7" si="8">LEN(A6)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M6" t="str">
         <f ca="1">CONCATENATE(C6,D6,E6,F6,G6,H6,I6)</f>
@@ -729,20 +728,20 @@
       </c>
       <c r="N6">
         <f ca="1">$J6+$K6+$M6+Q$10</f>
-        <v>2026373647</v>
+        <v>2023544356</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O7" ca="1" si="9">$J6*$K6+$M6+R$10</f>
-        <v>10111071069</v>
+        <f t="shared" ref="O6:O7" ca="1" si="8">$J6*$K6+$M6+R$10</f>
+        <v>40403670787</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="4">
-        <f t="shared" ref="Q6:R7" ca="1" si="10">MOD(N6,$B$2)</f>
-        <v>13100177</v>
+        <f t="shared" ref="Q6:R7" ca="1" si="9">MOD(N6,$B$2)</f>
+        <v>10270886</v>
       </c>
       <c r="R6" s="4">
-        <f t="shared" ca="1" si="10"/>
-        <v>13730281</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>14307635</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -782,12 +781,12 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="J7" si="10">LEN(A7)</f>
         <v>4</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M7" t="str">
         <f ca="1">CONCATENATE(C7,D7,E7,F7,G7,H7,I7)</f>
@@ -795,20 +794,20 @@
       </c>
       <c r="N7">
         <f t="shared" ref="N7" ca="1" si="11">$J7+$K7+$M7+Q$10</f>
-        <v>2038374926</v>
+        <v>2035545620</v>
       </c>
       <c r="O7">
-        <f t="shared" ca="1" si="9"/>
-        <v>8102979640</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8094188691</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="4">
-        <f t="shared" ca="1" si="10"/>
-        <v>9614737</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>6785431</v>
       </c>
       <c r="R7" s="4">
-        <f t="shared" ca="1" si="10"/>
-        <v>3425603</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10121373</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -819,10 +818,10 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q10" s="5">
         <f ca="1">RANDBETWEEN(1, $B$2)</f>
-        <v>6280613</v>
+        <v>3451305</v>
       </c>
       <c r="R10">
-        <v>10607204</v>
+        <v>1816247</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -909,7 +908,7 @@
       </c>
       <c r="K14" t="str">
         <f ca="1" xml:space="preserve"> TEXT(NOW(),"yyyymmddhh")</f>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M14" t="str">
         <f ca="1">CONCATENATE(C14,D14,E14,F14,G14,H14,I14)</f>
@@ -917,11 +916,11 @@
       </c>
       <c r="O14" s="2">
         <f t="shared" ref="O14" ca="1" si="13">M14+K14+J14+$Q$10</f>
-        <v>2027189647</v>
+        <v>2024360341</v>
       </c>
       <c r="Q14" s="5">
         <f ca="1">MOD(O14,$B$2)</f>
-        <v>13916177</v>
+        <v>11086871</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -966,7 +965,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" ref="K15:K17" ca="1" si="16" xml:space="preserve"> TEXT(NOW(),"yyyymmddhh")</f>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M15" t="str">
         <f ca="1">CONCATENATE(C15,D15,E15,F15,G15,H15,I15)</f>
@@ -975,11 +974,11 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2">
         <f ca="1">M15+K15+J15+$Q$10</f>
-        <v>2038853646</v>
+        <v>2036024340</v>
       </c>
       <c r="Q15" s="5">
         <f ca="1">MOD(O15,$B$2)</f>
-        <v>10093457</v>
+        <v>7264151</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1024,7 +1023,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M16" t="str">
         <f ca="1">CONCATENATE(C16,D16,E16,F16,G16,H16,I16)</f>
@@ -1032,11 +1031,11 @@
       </c>
       <c r="O16" s="2">
         <f t="shared" ref="O16:O17" ca="1" si="17">M16+K16+J16+$Q$10</f>
-        <v>2026373647</v>
+        <v>2023544341</v>
       </c>
       <c r="Q16" s="5">
         <f ca="1">MOD(O16,$B$2)</f>
-        <v>13100177</v>
+        <v>10270871</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1081,7 +1080,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>2020092709</v>
+        <v>2020092711</v>
       </c>
       <c r="M17" t="str">
         <f ca="1">CONCATENATE(C17,D17,E17,F17,G17,H17,I17)</f>
@@ -1089,11 +1088,11 @@
       </c>
       <c r="O17" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>2038374926</v>
+        <v>2035545620</v>
       </c>
       <c r="Q17" s="5">
         <f ca="1">MOD(O17,$B$2)</f>
-        <v>9614737</v>
+        <v>6785431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>